<commit_message>
swapped CRISP and ImLock wavelengths
</commit_message>
<xml_diff>
--- a/Parts-List/FocusShifter-Parts.xlsx
+++ b/Parts-List/FocusShifter-Parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshe\Documents\GitHub\LifeHackWebsite\Parts-List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D7776-2B08-4E88-BF7D-484CEEFA0882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FE935B-6A1F-4333-9D7F-65EFE9CF189A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D35111BA-CF0D-4FF5-85D4-DC133290B806}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D35111BA-CF0D-4FF5-85D4-DC133290B806}"/>
   </bookViews>
   <sheets>
     <sheet name="Focus Shifter" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,6 @@
     <t>CRISP-5 ASSEMBLY</t>
   </si>
   <si>
-    <t>DASI/CRISP-850</t>
-  </si>
-  <si>
-    <t>Cairn research</t>
-  </si>
-  <si>
     <t>zoom-tube-lens</t>
   </si>
   <si>
@@ -268,6 +262,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>ASI</t>
+  </si>
+  <si>
+    <t>DASI/CRISP-940</t>
   </si>
 </sst>
 </file>
@@ -660,26 +660,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0C5541-9F2E-4046-980B-8593A33110BF}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="7" max="7" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -702,15 +702,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -724,22 +724,22 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -752,15 +752,15 @@
         <v>161.51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -773,22 +773,22 @@
         <v>42.81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -801,15 +801,15 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -822,15 +822,15 @@
         <v>26.72</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -843,15 +843,15 @@
         <v>30.84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -864,22 +864,22 @@
         <v>21.71</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -892,15 +892,15 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -913,15 +913,15 @@
         <v>8.77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -934,22 +934,22 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -962,15 +962,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -983,15 +983,15 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1004,22 +1004,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1032,15 +1032,15 @@
         <v>6.18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1054,22 +1054,22 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1082,15 +1082,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>1438</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1103,15 +1103,15 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" s="2">
         <v>0.747</v>
@@ -1121,15 +1121,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1142,15 +1142,15 @@
         <v>11.85</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1163,15 +1163,15 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
         <v>57</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1184,15 +1184,15 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1205,15 +1205,15 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1227,15 +1227,15 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1248,15 +1248,15 @@
         <v>11.52</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1269,15 +1269,15 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1290,15 +1290,15 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1311,15 +1311,15 @@
         <v>6.42</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1333,15 +1333,15 @@
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1355,15 +1355,15 @@
       </c>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1377,9 +1377,9 @@
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F41" s="2">
         <f>SUM(F3:F38)</f>

</xml_diff>